<commit_message>
Created centrality injection function
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,22 +454,30 @@
           <t>Population-Weighted Centrality Infection via Delta</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Centrality-Infection via Injection vs. Uniform</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5</v>
+        <v>0.630878852342418</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5</v>
+        <v>0.630878852342418</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5</v>
+        <v>0.630878852342418</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5</v>
+        <v>0.630878852342418</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.630878852342418</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +485,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.504640832930681</v>
+        <v>0.6310585891651432</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4956696324074922</v>
+        <v>0.6309249401054441</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4849637190004192</v>
+        <v>0.6315599155696284</v>
       </c>
       <c r="E3" t="n">
-        <v>0.509638906593664</v>
+        <v>0.6313602110834218</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6306956250281268</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +505,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5036789907368531</v>
+        <v>0.6312119834750214</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4892099140249971</v>
+        <v>0.631373119989129</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4781844546173888</v>
+        <v>0.6321126582957415</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5012823466591082</v>
+        <v>0.6317919579145712</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6301326055878808</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +525,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4995680209475696</v>
+        <v>0.6320040164391563</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4935553248647283</v>
+        <v>0.6312350581624695</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4815347877794992</v>
+        <v>0.6321159330358305</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5180828799648001</v>
+        <v>0.6322191748176234</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6293634570187543</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +545,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4954132194880937</v>
+        <v>0.6323533091113186</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4915826709398864</v>
+        <v>0.6310795751901689</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4887846424317741</v>
+        <v>0.6320984050558672</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5170554424988971</v>
+        <v>0.6329260698705839</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.6284815277442427</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +565,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4956074084433689</v>
+        <v>0.6327424061180165</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4917209401999541</v>
+        <v>0.6317737918834813</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4899773519739932</v>
+        <v>0.6324870890879113</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5262954330113201</v>
+        <v>0.6336606340372738</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6275243667158602</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +585,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4980990565196244</v>
+        <v>0.632628258233615</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4994471144584595</v>
+        <v>0.6321728255078607</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4833861222074002</v>
+        <v>0.6326156988599391</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5363029113644051</v>
+        <v>0.6343034105146113</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6265209489400879</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +605,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4957841630892545</v>
+        <v>0.6332525531843466</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5058543961003844</v>
+        <v>0.6328424527778863</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4826513522744099</v>
+        <v>0.6327856082528848</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5391282709778005</v>
+        <v>0.6348266914502152</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.6254938097747909</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +625,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5019175425332829</v>
+        <v>0.6335869724084373</v>
       </c>
       <c r="C10" t="n">
-        <v>0.506801687286038</v>
+        <v>0.6329502410099481</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4872675313381081</v>
+        <v>0.6331517088875707</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5501665838876781</v>
+        <v>0.6353464056220384</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.6244587360111407</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +645,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5033922635750263</v>
+        <v>0.6337939645697725</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5162690530604233</v>
+        <v>0.6329981907347569</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4862165177555541</v>
+        <v>0.6332842821943229</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5522644787356377</v>
+        <v>0.6358377886284368</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.62340490699346</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +665,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5000783342856926</v>
+        <v>0.6343790088994058</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5156586948021534</v>
+        <v>0.6334329973842313</v>
       </c>
       <c r="D12" t="n">
-        <v>0.485764114801632</v>
+        <v>0.6335576994449355</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5512197590061485</v>
+        <v>0.6363963024477666</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6223372515950404</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +685,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5029645063443006</v>
+        <v>0.6342597873311659</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5112213235159354</v>
+        <v>0.6335394359604829</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4913457972630949</v>
+        <v>0.6334804547237531</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5561890920367576</v>
+        <v>0.636966907939407</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.621278791782906</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +705,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4989658571259988</v>
+        <v>0.6343724362630584</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5178943730908323</v>
+        <v>0.6337840106334115</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4972854889878945</v>
+        <v>0.6332848938641013</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5570182274797364</v>
+        <v>0.6371847635847345</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6202277780089492</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +725,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5036790310014096</v>
+        <v>0.634392725768963</v>
       </c>
       <c r="C15" t="n">
-        <v>0.519127255009221</v>
+        <v>0.634180425793528</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4989009200356665</v>
+        <v>0.6330196427055196</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5617334866813632</v>
+        <v>0.6376115181679561</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.6191634819463486</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +745,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5066918865986475</v>
+        <v>0.634280797191882</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5167423781088321</v>
+        <v>0.6344823188062695</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4960220843513339</v>
+        <v>0.6327957453726237</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5644951676017096</v>
+        <v>0.6380999925546399</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.6181191448545947</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +765,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5059553347244371</v>
+        <v>0.6347335748847958</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5171160856627657</v>
+        <v>0.6345869819892926</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4981968725524153</v>
+        <v>0.6328974400000684</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5695248615357078</v>
+        <v>0.6384918538502624</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6170805350332741</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +785,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5056755544514765</v>
+        <v>0.6349879593174956</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5191284276761253</v>
+        <v>0.6352327626318613</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4959909157546878</v>
+        <v>0.6331040858797287</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5732333823186241</v>
+        <v>0.6392028537523683</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6160488233628796</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +805,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5045561484323152</v>
+        <v>0.6350261943435054</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5254673310095346</v>
+        <v>0.635501685393544</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4963807759888924</v>
+        <v>0.6334637004948123</v>
       </c>
       <c r="E19" t="n">
-        <v>0.575722093268429</v>
+        <v>0.6393312137670005</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.6150280386447374</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +825,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5047230158425851</v>
+        <v>0.6349861482955065</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5280346297549283</v>
+        <v>0.6358067383016467</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4985736978053739</v>
+        <v>0.6334386874926429</v>
       </c>
       <c r="E20" t="n">
-        <v>0.57659525263212</v>
+        <v>0.6400637850800956</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.6140073679240082</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +845,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5062099048329594</v>
+        <v>0.6349056461287013</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5342377120819682</v>
+        <v>0.6358927283391898</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5016815488499113</v>
+        <v>0.6332204114392054</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5793006239890325</v>
+        <v>0.6405828707979337</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.6129893340347664</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +865,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.5093087845682479</v>
+        <v>0.6346835072871099</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5363900998486989</v>
+        <v>0.636595841160375</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5008714910776394</v>
+        <v>0.633243382537557</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5804736410583184</v>
+        <v>0.6409347623387822</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.6119964118821827</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +885,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.5065840022377995</v>
+        <v>0.6349183424965422</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5390765229805996</v>
+        <v>0.6369561637789384</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4997725883864577</v>
+        <v>0.633151814363234</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5821768369961919</v>
+        <v>0.6413562686558067</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.6110100375320124</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +905,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5088339477569808</v>
+        <v>0.6349015160433645</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5428137663694631</v>
+        <v>0.6375631313890157</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5025241346184994</v>
+        <v>0.6330901017797299</v>
       </c>
       <c r="E24" t="n">
-        <v>0.584450183083191</v>
+        <v>0.6420645910912204</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.6100266534821943</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +925,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.5071117187499306</v>
+        <v>0.63535973463038</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5460301792054917</v>
+        <v>0.6381132890173717</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5030067459775364</v>
+        <v>0.6331554478152714</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5806891696659873</v>
+        <v>0.6425753085529051</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.6090557735644599</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +945,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.5053535804204154</v>
+        <v>0.6353153893565116</v>
       </c>
       <c r="C26" t="n">
-        <v>0.546172213284161</v>
+        <v>0.6386228189420139</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5001703970789293</v>
+        <v>0.6327083569997961</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5816070816091486</v>
+        <v>0.643124144126124</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.6080992450366451</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +965,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.5041242486272517</v>
+        <v>0.6352745529661502</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5504880799624748</v>
+        <v>0.6392598722755387</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5016340903730395</v>
+        <v>0.6325668492167864</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5826038648174743</v>
+        <v>0.6437745654108056</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.6071582283242362</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +985,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.5071633347421572</v>
+        <v>0.6352480752466734</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5505887339971313</v>
+        <v>0.6398745625474433</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5007719315034349</v>
+        <v>0.6321780762729013</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5823797498301364</v>
+        <v>0.644083281963743</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.6062151105345934</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +1005,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.5049826829991525</v>
+        <v>0.6351889043720489</v>
       </c>
       <c r="C29" t="n">
-        <v>0.5518920427214236</v>
+        <v>0.6402125247984314</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4985339689536401</v>
+        <v>0.6320811575709037</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5866033236960783</v>
+        <v>0.6441627243236534</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.6052870623422187</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +1025,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.5037575671010104</v>
+        <v>0.6352540826650774</v>
       </c>
       <c r="C30" t="n">
-        <v>0.5560942866584645</v>
+        <v>0.6409045641655653</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4982720405755542</v>
+        <v>0.6320488201680599</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5869785802250196</v>
+        <v>0.6444563914893908</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.6043650501416171</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +1045,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.5059563396064111</v>
+        <v>0.6352408500664309</v>
       </c>
       <c r="C31" t="n">
-        <v>0.5586709782791104</v>
+        <v>0.6410778540390391</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4979702662563016</v>
+        <v>0.6320417507587598</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5866353017642097</v>
+        <v>0.6451798765768817</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.6034563016289947</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +1065,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.5046531245917271</v>
+        <v>0.6353145549390261</v>
       </c>
       <c r="C32" t="n">
-        <v>0.5615505459608104</v>
+        <v>0.6414421719657201</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4966644268491432</v>
+        <v>0.6318527786129804</v>
       </c>
       <c r="E32" t="n">
-        <v>0.585867145749837</v>
+        <v>0.6456522498884918</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.6025561213023591</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +1085,19 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.5034398078851838</v>
+        <v>0.6355611917721994</v>
       </c>
       <c r="C33" t="n">
-        <v>0.5629811285954431</v>
+        <v>0.641804560083699</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4967844482953342</v>
+        <v>0.6316601270029523</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5879845729793378</v>
+        <v>0.6461424029238177</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.6016669091976461</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1105,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.5022866005022085</v>
+        <v>0.635628713076571</v>
       </c>
       <c r="C34" t="n">
-        <v>0.562566946231114</v>
+        <v>0.6421668366581066</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4983347316095885</v>
+        <v>0.6316850995864816</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5875971304257357</v>
+        <v>0.6465679443667114</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.6007802106231416</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1125,19 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5019757446391644</v>
+        <v>0.6354191496283587</v>
       </c>
       <c r="C35" t="n">
-        <v>0.5632949316722415</v>
+        <v>0.6426297743520429</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4982072561025722</v>
+        <v>0.6314722863356625</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5861321509467331</v>
+        <v>0.6469051071280411</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.5999050087919133</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1145,19 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5035786443457094</v>
+        <v>0.6354048542237002</v>
       </c>
       <c r="C36" t="n">
-        <v>0.5644661540193743</v>
+        <v>0.6432617265196904</v>
       </c>
       <c r="D36" t="n">
-        <v>0.4996210087251151</v>
+        <v>0.6314298449557207</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5875681604704874</v>
+        <v>0.6473562709076421</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.5990383772874347</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1165,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.502610350454202</v>
+        <v>0.6355268946324392</v>
       </c>
       <c r="C37" t="n">
-        <v>0.567151298793621</v>
+        <v>0.6436438803624799</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4984979957264856</v>
+        <v>0.6313450382467641</v>
       </c>
       <c r="E37" t="n">
-        <v>0.5869516457100066</v>
+        <v>0.6477720955097158</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.5981888452158264</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1185,19 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.503103307948352</v>
+        <v>0.6356277008257571</v>
       </c>
       <c r="C38" t="n">
-        <v>0.5684557902973331</v>
+        <v>0.6439001060573319</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4971525800452164</v>
+        <v>0.6314365480120233</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5870253259869825</v>
+        <v>0.6480131888017006</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.5973474018940912</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1205,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.5044616913039658</v>
+        <v>0.6356756486210895</v>
       </c>
       <c r="C39" t="n">
-        <v>0.5695257667457202</v>
+        <v>0.6441274575362907</v>
       </c>
       <c r="D39" t="n">
-        <v>0.4992612209395073</v>
+        <v>0.6312981638395959</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5884292569977653</v>
+        <v>0.6486226003147093</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.5965190536338605</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1225,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5055303359483284</v>
+        <v>0.6359668686965814</v>
       </c>
       <c r="C40" t="n">
-        <v>0.5729204169023244</v>
+        <v>0.6446120491400621</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5012119130074526</v>
+        <v>0.6311067129999889</v>
       </c>
       <c r="E40" t="n">
-        <v>0.588224554518778</v>
+        <v>0.6495465737929675</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.5956904891592723</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1245,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.5087605703019084</v>
+        <v>0.6362800130747455</v>
       </c>
       <c r="C41" t="n">
-        <v>0.5731268427474284</v>
+        <v>0.6449235325335498</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5015120347832961</v>
+        <v>0.6308953541399142</v>
       </c>
       <c r="E41" t="n">
-        <v>0.587307794735304</v>
+        <v>0.6500311999399144</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.594870952502616</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1265,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.5100220934648523</v>
+        <v>0.6364464373555277</v>
       </c>
       <c r="C42" t="n">
-        <v>0.5750392421458056</v>
+        <v>0.6450623892964118</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5036559618619347</v>
+        <v>0.6307896866178527</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5875194413599339</v>
+        <v>0.6505709203575366</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.5940548858513132</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1285,19 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.5089861101109829</v>
+        <v>0.6364946091034486</v>
       </c>
       <c r="C43" t="n">
-        <v>0.5754839832494404</v>
+        <v>0.6457483076630754</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5026636288565244</v>
+        <v>0.630607139535135</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5893298052108432</v>
+        <v>0.6509067166518846</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.5932485956412232</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1305,19 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.5099335533507904</v>
+        <v>0.636673020600795</v>
       </c>
       <c r="C44" t="n">
-        <v>0.5769375477805198</v>
+        <v>0.6460504037490493</v>
       </c>
       <c r="D44" t="n">
-        <v>0.5034272374047992</v>
+        <v>0.6304520375148479</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5921192349404583</v>
+        <v>0.6510399449245653</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.5924493436622028</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1325,19 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.5114042902461937</v>
+        <v>0.6367559852873217</v>
       </c>
       <c r="C45" t="n">
-        <v>0.5774909722197827</v>
+        <v>0.6466988627355768</v>
       </c>
       <c r="D45" t="n">
-        <v>0.5054249246724154</v>
+        <v>0.6303868365639558</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5934850318382776</v>
+        <v>0.6511660635099389</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.5916620399993235</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1345,19 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.510257026602026</v>
+        <v>0.6365898316032431</v>
       </c>
       <c r="C46" t="n">
-        <v>0.5780322376800845</v>
+        <v>0.6471524252849423</v>
       </c>
       <c r="D46" t="n">
-        <v>0.506078264770115</v>
+        <v>0.6300733169748387</v>
       </c>
       <c r="E46" t="n">
-        <v>0.5941246526095223</v>
+        <v>0.6513572727665312</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.5908867324282142</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1365,19 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.5108493967159526</v>
+        <v>0.6366093260122286</v>
       </c>
       <c r="C47" t="n">
-        <v>0.5780702413315193</v>
+        <v>0.647342411486262</v>
       </c>
       <c r="D47" t="n">
-        <v>0.5065236674714446</v>
+        <v>0.6298149422859626</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5924587230176666</v>
+        <v>0.6516951644006419</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.5901162395273585</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1385,19 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.5097884544911078</v>
+        <v>0.6367299748191142</v>
       </c>
       <c r="C48" t="n">
-        <v>0.5778915851829984</v>
+        <v>0.6475625165422021</v>
       </c>
       <c r="D48" t="n">
-        <v>0.5063293912299812</v>
+        <v>0.6297632554119877</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5924087007469542</v>
+        <v>0.6520147502889413</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.589353933688186</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1405,19 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.5092479520544313</v>
+        <v>0.6366350659325017</v>
       </c>
       <c r="C49" t="n">
-        <v>0.5785824900693202</v>
+        <v>0.6478510963923022</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5042547534828123</v>
+        <v>0.6298597933110768</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5937259244785738</v>
+        <v>0.6523899885101281</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.5886023298667997</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1425,19 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.5092401874375349</v>
+        <v>0.6368887698829995</v>
       </c>
       <c r="C50" t="n">
-        <v>0.579485813939111</v>
+        <v>0.6486039384393552</v>
       </c>
       <c r="D50" t="n">
-        <v>0.5035729408904676</v>
+        <v>0.6298699404342788</v>
       </c>
       <c r="E50" t="n">
-        <v>0.5935429996886769</v>
+        <v>0.6526215235882147</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.5878493489316882</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1445,19 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.5091796971273015</v>
+        <v>0.6369562665306046</v>
       </c>
       <c r="C51" t="n">
-        <v>0.578861272482083</v>
+        <v>0.6489821249076566</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5040981876349935</v>
+        <v>0.6299143487985035</v>
       </c>
       <c r="E51" t="n">
-        <v>0.594136656000419</v>
+        <v>0.6527669384801909</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.5871152003518355</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1465,19 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.5108726759822121</v>
+        <v>0.6370661331461875</v>
       </c>
       <c r="C52" t="n">
-        <v>0.5802605843096698</v>
+        <v>0.6492266399668403</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5042375369153108</v>
+        <v>0.6297123554957661</v>
       </c>
       <c r="E52" t="n">
-        <v>0.5942489878967475</v>
+        <v>0.653077156610133</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.5863775398736866</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1485,19 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.5080049904028771</v>
+        <v>0.6368259819870878</v>
       </c>
       <c r="C53" t="n">
-        <v>0.5804706360499214</v>
+        <v>0.6494148885562964</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5051091381989623</v>
+        <v>0.6295011234946088</v>
       </c>
       <c r="E53" t="n">
-        <v>0.5945873891284952</v>
+        <v>0.6533551432165171</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.5856477127947226</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1505,19 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.5092439043319892</v>
+        <v>0.6366737366510871</v>
       </c>
       <c r="C54" t="n">
-        <v>0.5808452358657064</v>
+        <v>0.6500087755594885</v>
       </c>
       <c r="D54" t="n">
-        <v>0.5055655850647975</v>
+        <v>0.6294865522551275</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5953897565161159</v>
+        <v>0.6536268028682753</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.5849285396823288</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1525,19 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.509142172185135</v>
+        <v>0.6367922362978619</v>
       </c>
       <c r="C55" t="n">
-        <v>0.5808091069580595</v>
+        <v>0.650306807624035</v>
       </c>
       <c r="D55" t="n">
-        <v>0.506214571450245</v>
+        <v>0.6293484852864645</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5967538589221324</v>
+        <v>0.6541246316576692</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.5842218909392481</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1545,19 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.5087766371619437</v>
+        <v>0.6366892250251612</v>
       </c>
       <c r="C56" t="n">
-        <v>0.5804127871319725</v>
+        <v>0.6507989190491947</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5072290988369603</v>
+        <v>0.6294980582233304</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5951812244524169</v>
+        <v>0.6544518505827387</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.5835195075899176</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1565,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.5068823343006856</v>
+        <v>0.6366983507144918</v>
       </c>
       <c r="C57" t="n">
-        <v>0.5817755408126243</v>
+        <v>0.6511099244358989</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5086050635741909</v>
+        <v>0.6293011123570132</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5960645313745829</v>
+        <v>0.6544176741749409</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.5828199344924478</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1585,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.5051243089155716</v>
+        <v>0.6368678076037506</v>
       </c>
       <c r="C58" t="n">
-        <v>0.5820810003856447</v>
+        <v>0.6515045437219324</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5081386082831256</v>
+        <v>0.6293895266832347</v>
       </c>
       <c r="E58" t="n">
-        <v>0.596090080238852</v>
+        <v>0.654802481857005</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.5821275458337482</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1605,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.5046246549707553</v>
+        <v>0.636854568359246</v>
       </c>
       <c r="C59" t="n">
-        <v>0.5838522398818315</v>
+        <v>0.6517053143900928</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5091948531076216</v>
+        <v>0.6293533507283616</v>
       </c>
       <c r="E59" t="n">
-        <v>0.5961003235384</v>
+        <v>0.6554238765369282</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.5814435108736371</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1625,19 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.5031638191177594</v>
+        <v>0.6369902823352166</v>
       </c>
       <c r="C60" t="n">
-        <v>0.5845966310545821</v>
+        <v>0.6519651648912059</v>
       </c>
       <c r="D60" t="n">
-        <v>0.5100957574666605</v>
+        <v>0.6292798097341825</v>
       </c>
       <c r="E60" t="n">
-        <v>0.5960371678899323</v>
+        <v>0.6559319272631595</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.5807672944559056</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1645,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.5041192232591568</v>
+        <v>0.6369527151558715</v>
       </c>
       <c r="C61" t="n">
-        <v>0.5852418581381784</v>
+        <v>0.6524420533186657</v>
       </c>
       <c r="D61" t="n">
-        <v>0.510890076867293</v>
+        <v>0.6292429441993492</v>
       </c>
       <c r="E61" t="n">
-        <v>0.5970981700843054</v>
+        <v>0.6563146294261589</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.5800994866279309</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1665,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.5031528285465346</v>
+        <v>0.6370189202955581</v>
       </c>
       <c r="C62" t="n">
-        <v>0.5872106633905694</v>
+        <v>0.6529019023052897</v>
       </c>
       <c r="D62" t="n">
-        <v>0.509325570474962</v>
+        <v>0.6291712183673999</v>
       </c>
       <c r="E62" t="n">
-        <v>0.5973712496431709</v>
+        <v>0.656645210431582</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.5794276332936101</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1685,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.5025378802871885</v>
+        <v>0.6371905051152424</v>
       </c>
       <c r="C63" t="n">
-        <v>0.5881428749518853</v>
+        <v>0.6534082490678331</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5090822227850584</v>
+        <v>0.6292776841903523</v>
       </c>
       <c r="E63" t="n">
-        <v>0.597952378678422</v>
+        <v>0.6568818715655397</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.5787661148732463</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1705,19 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.5026477438780732</v>
+        <v>0.6373636237773658</v>
       </c>
       <c r="C64" t="n">
-        <v>0.5886208266961158</v>
+        <v>0.6539516704408588</v>
       </c>
       <c r="D64" t="n">
-        <v>0.5097010781794923</v>
+        <v>0.6290206702656553</v>
       </c>
       <c r="E64" t="n">
-        <v>0.5987474763287652</v>
+        <v>0.6572478198593931</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.5781137215915997</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1725,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.5045679867576716</v>
+        <v>0.6374636637528882</v>
       </c>
       <c r="C65" t="n">
-        <v>0.5892795285285685</v>
+        <v>0.6542966446658556</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5104038508758799</v>
+        <v>0.628836900695014</v>
       </c>
       <c r="E65" t="n">
-        <v>0.5996237469111211</v>
+        <v>0.6576375019951954</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.5774621908921789</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1745,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.5041017113877415</v>
+        <v>0.6374769176353848</v>
       </c>
       <c r="C66" t="n">
-        <v>0.5900598535754107</v>
+        <v>0.6544576767367876</v>
       </c>
       <c r="D66" t="n">
-        <v>0.5122176076819372</v>
+        <v>0.6286418379505998</v>
       </c>
       <c r="E66" t="n">
-        <v>0.6001836607906346</v>
+        <v>0.657880287959129</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.5768208422312989</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1765,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.5050022208484897</v>
+        <v>0.6372630154287025</v>
       </c>
       <c r="C67" t="n">
-        <v>0.5902789609605894</v>
+        <v>0.6547610530089683</v>
       </c>
       <c r="D67" t="n">
-        <v>0.5131769548959003</v>
+        <v>0.6284289200365363</v>
       </c>
       <c r="E67" t="n">
-        <v>0.6004437310354888</v>
+        <v>0.6582330051208926</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.5761845988528653</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1785,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.5055280183733987</v>
+        <v>0.6371576984421299</v>
       </c>
       <c r="C68" t="n">
-        <v>0.5910955654744663</v>
+        <v>0.6550918249286666</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5134770261418575</v>
+        <v>0.6282973764380311</v>
       </c>
       <c r="E68" t="n">
-        <v>0.6003539867340304</v>
+        <v>0.6587504120847428</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.5755541068171344</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1805,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.5060048079840911</v>
+        <v>0.6369924927114973</v>
       </c>
       <c r="C69" t="n">
-        <v>0.592324061456066</v>
+        <v>0.6554133050270234</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5134131353824188</v>
+        <v>0.6282391219617259</v>
       </c>
       <c r="E69" t="n">
-        <v>0.6015262771881529</v>
+        <v>0.6590097301245551</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.5749342219820961</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1825,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.5043504109035166</v>
+        <v>0.6369168363999524</v>
       </c>
       <c r="C70" t="n">
-        <v>0.5932413107351757</v>
+        <v>0.655634342615892</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5143218778045265</v>
+        <v>0.6280929999944498</v>
       </c>
       <c r="E70" t="n">
-        <v>0.6033640125062719</v>
+        <v>0.6591795631998244</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.5743188454163592</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1845,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.5050370140254651</v>
+        <v>0.6371299858360751</v>
       </c>
       <c r="C71" t="n">
-        <v>0.5929881846945158</v>
+        <v>0.655955394854128</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5140912212451793</v>
+        <v>0.6279535529395133</v>
       </c>
       <c r="E71" t="n">
-        <v>0.6035959845675805</v>
+        <v>0.6595869226539766</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.5737052910364906</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1865,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5060103356142684</v>
+        <v>0.6372535763480162</v>
       </c>
       <c r="C72" t="n">
-        <v>0.5933933389503733</v>
+        <v>0.6561163492499575</v>
       </c>
       <c r="D72" t="n">
-        <v>0.5146422100493162</v>
+        <v>0.6277515603843234</v>
       </c>
       <c r="E72" t="n">
-        <v>0.6038377231979931</v>
+        <v>0.6597642155973953</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.5731015346499864</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1885,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.5063098173416838</v>
+        <v>0.6370596599758789</v>
       </c>
       <c r="C73" t="n">
-        <v>0.5937752154621248</v>
+        <v>0.6563988098568238</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5147909773090602</v>
+        <v>0.6275585782344187</v>
       </c>
       <c r="E73" t="n">
-        <v>0.6034548358910915</v>
+        <v>0.660049607168258</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.5724992103279428</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1905,19 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.5072236753251003</v>
+        <v>0.6369683078319476</v>
       </c>
       <c r="C74" t="n">
-        <v>0.594084755919517</v>
+        <v>0.6566938899074541</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5144044209267734</v>
+        <v>0.6276275921303689</v>
       </c>
       <c r="E74" t="n">
-        <v>0.6039236822658266</v>
+        <v>0.6602111338176693</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.5719064252310033</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1925,19 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.5076592263678463</v>
+        <v>0.6370754092750028</v>
       </c>
       <c r="C75" t="n">
-        <v>0.5945513560628968</v>
+        <v>0.6570198485100732</v>
       </c>
       <c r="D75" t="n">
-        <v>0.5145046661444383</v>
+        <v>0.6275353876453927</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6053296980287867</v>
+        <v>0.6604736807355536</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.5713145052824669</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1945,19 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.5091625900092935</v>
+        <v>0.6371215232242259</v>
       </c>
       <c r="C76" t="n">
-        <v>0.5943914510206441</v>
+        <v>0.6572498791977135</v>
       </c>
       <c r="D76" t="n">
-        <v>0.513864597861566</v>
+        <v>0.6272762755253296</v>
       </c>
       <c r="E76" t="n">
-        <v>0.6053815715595302</v>
+        <v>0.6607556293087279</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.5707278592053272</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1965,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.5097843040381049</v>
+        <v>0.6372029893388738</v>
       </c>
       <c r="C77" t="n">
-        <v>0.5947210128159177</v>
+        <v>0.6574247595260483</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5133555295312096</v>
+        <v>0.6272251291666027</v>
       </c>
       <c r="E77" t="n">
-        <v>0.6071293325635304</v>
+        <v>0.6611109494056353</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.5701481686885634</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1985,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.5106304267477297</v>
+        <v>0.6373110995556363</v>
       </c>
       <c r="C78" t="n">
-        <v>0.5959054435932636</v>
+        <v>0.6576907434919719</v>
       </c>
       <c r="D78" t="n">
-        <v>0.5126496774619748</v>
+        <v>0.6272708899179467</v>
       </c>
       <c r="E78" t="n">
-        <v>0.6069938966429589</v>
+        <v>0.661549634408384</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.5695733091183645</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +2005,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.5104748391680463</v>
+        <v>0.6374693813286844</v>
       </c>
       <c r="C79" t="n">
-        <v>0.5965856055714494</v>
+        <v>0.6579411156655357</v>
       </c>
       <c r="D79" t="n">
-        <v>0.5115466269237033</v>
+        <v>0.6271712334306661</v>
       </c>
       <c r="E79" t="n">
-        <v>0.6070686396260557</v>
+        <v>0.6617669065845345</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.5690029874870386</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +2025,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.5114365646886961</v>
+        <v>0.6376757810079864</v>
       </c>
       <c r="C80" t="n">
-        <v>0.5968851379975495</v>
+        <v>0.6582382874269352</v>
       </c>
       <c r="D80" t="n">
-        <v>0.5106630176412514</v>
+        <v>0.6272007032779628</v>
       </c>
       <c r="E80" t="n">
-        <v>0.6076530088593318</v>
+        <v>0.6621116870700239</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.5684325626406105</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +2045,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.51063413682922</v>
+        <v>0.6377115111735543</v>
       </c>
       <c r="C81" t="n">
-        <v>0.597467106651647</v>
+        <v>0.65848672090727</v>
       </c>
       <c r="D81" t="n">
-        <v>0.5117103879436238</v>
+        <v>0.6271887917577162</v>
       </c>
       <c r="E81" t="n">
-        <v>0.6081839959357135</v>
+        <v>0.6624099011247617</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.5678706664161054</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +2065,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.5105435922779041</v>
+        <v>0.6377568458673686</v>
       </c>
       <c r="C82" t="n">
-        <v>0.5983742642492056</v>
+        <v>0.6586755716325698</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5115101810832305</v>
+        <v>0.6268926795646512</v>
       </c>
       <c r="E82" t="n">
-        <v>0.6077043356212307</v>
+        <v>0.6629070277812948</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.5673135722049414</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +2085,19 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.5107939217613515</v>
+        <v>0.637704408256337</v>
       </c>
       <c r="C83" t="n">
-        <v>0.5994445386644867</v>
+        <v>0.6590405747895415</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5109707979929975</v>
+        <v>0.6267187752967848</v>
       </c>
       <c r="E83" t="n">
-        <v>0.6078086886055434</v>
+        <v>0.6632091206280963</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.5667590843342886</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +2105,19 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.5110417384224274</v>
+        <v>0.6376824320606409</v>
       </c>
       <c r="C84" t="n">
-        <v>0.5988512974768005</v>
+        <v>0.6593643948775657</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5119837629973329</v>
+        <v>0.6266162910691584</v>
       </c>
       <c r="E84" t="n">
-        <v>0.6082474943336035</v>
+        <v>0.6635750521055771</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.5662125034177181</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +2125,19 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.5122458731318946</v>
+        <v>0.6377415029299195</v>
       </c>
       <c r="C85" t="n">
-        <v>0.6000242432967908</v>
+        <v>0.6595179771347741</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5123936455090988</v>
+        <v>0.6265428041023836</v>
       </c>
       <c r="E85" t="n">
-        <v>0.6076432878910447</v>
+        <v>0.6638125262541075</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.5656725878744817</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +2145,19 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.5118712713418792</v>
+        <v>0.6378557492498238</v>
       </c>
       <c r="C86" t="n">
-        <v>0.5997489134677179</v>
+        <v>0.6596113740472797</v>
       </c>
       <c r="D86" t="n">
-        <v>0.512317031921484</v>
+        <v>0.6265099661510557</v>
       </c>
       <c r="E86" t="n">
-        <v>0.6088870077581024</v>
+        <v>0.663899662959711</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.5651366306851429</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +2165,19 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.5110158076279184</v>
+        <v>0.6378184642802815</v>
       </c>
       <c r="C87" t="n">
-        <v>0.5999337613118152</v>
+        <v>0.6600217690673771</v>
       </c>
       <c r="D87" t="n">
-        <v>0.512488302859336</v>
+        <v>0.6264404666467231</v>
       </c>
       <c r="E87" t="n">
-        <v>0.6097210024201936</v>
+        <v>0.6640534331454753</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.5646045120031581</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +2185,19 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.5108204973234691</v>
+        <v>0.6379719115160819</v>
       </c>
       <c r="C88" t="n">
-        <v>0.6001074360874515</v>
+        <v>0.6600642962553667</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5119083839969584</v>
+        <v>0.6261591165365105</v>
       </c>
       <c r="E88" t="n">
-        <v>0.6087970705804361</v>
+        <v>0.664204878811406</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.5640785321918552</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +2205,19 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5116548769617828</v>
+        <v>0.6379408718838194</v>
       </c>
       <c r="C89" t="n">
-        <v>0.6007196237013461</v>
+        <v>0.6604892664218734</v>
       </c>
       <c r="D89" t="n">
-        <v>0.5107348361264944</v>
+        <v>0.6259341424303331</v>
       </c>
       <c r="E89" t="n">
-        <v>0.6089352280027105</v>
+        <v>0.6643932862230798</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.5635519564934364</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +2225,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.5118095884191812</v>
+        <v>0.6379227131848999</v>
       </c>
       <c r="C90" t="n">
-        <v>0.6019096669351433</v>
+        <v>0.6607980699824443</v>
       </c>
       <c r="D90" t="n">
-        <v>0.510563207705881</v>
+        <v>0.6259085551015373</v>
       </c>
       <c r="E90" t="n">
-        <v>0.6093834406360916</v>
+        <v>0.6644368587715392</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.563031008921398</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +2245,19 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.511270762342433</v>
+        <v>0.638068707657834</v>
       </c>
       <c r="C91" t="n">
-        <v>0.6021116426072732</v>
+        <v>0.6609867829730295</v>
       </c>
       <c r="D91" t="n">
-        <v>0.5116134322371282</v>
+        <v>0.6256848358308332</v>
       </c>
       <c r="E91" t="n">
-        <v>0.6098941857529632</v>
+        <v>0.6647910485820989</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.5625122534061411</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +2265,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.5113010077758301</v>
+        <v>0.6382088100157972</v>
       </c>
       <c r="C92" t="n">
-        <v>0.6025922606295711</v>
+        <v>0.6610925358597923</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5111094195284799</v>
+        <v>0.6255902318070127</v>
       </c>
       <c r="E92" t="n">
-        <v>0.6108494694951081</v>
+        <v>0.6651000245318541</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.5619998013382876</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2285,19 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.5113650273705979</v>
+        <v>0.6382817112055233</v>
       </c>
       <c r="C93" t="n">
-        <v>0.6028285900573683</v>
+        <v>0.6613159209303332</v>
       </c>
       <c r="D93" t="n">
-        <v>0.5122957754774096</v>
+        <v>0.6253142726033822</v>
       </c>
       <c r="E93" t="n">
-        <v>0.6116013158798618</v>
+        <v>0.6652512908671394</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.5614934018660606</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2305,19 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.5103680696751356</v>
+        <v>0.6383977437907771</v>
       </c>
       <c r="C94" t="n">
-        <v>0.603705920733565</v>
+        <v>0.6616716006339802</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5137312614386742</v>
+        <v>0.625083457461758</v>
       </c>
       <c r="E94" t="n">
-        <v>0.6115731372885287</v>
+        <v>0.6654885016819907</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.5609855315434485</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2325,19 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.5106771841213955</v>
+        <v>0.638516463205692</v>
       </c>
       <c r="C95" t="n">
-        <v>0.6045391464751395</v>
+        <v>0.6620227922843264</v>
       </c>
       <c r="D95" t="n">
-        <v>0.512776714489881</v>
+        <v>0.6250242537585416</v>
       </c>
       <c r="E95" t="n">
-        <v>0.612628818415909</v>
+        <v>0.6657408380257294</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.5604865377199633</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2345,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5100410441642234</v>
+        <v>0.6386935603297377</v>
       </c>
       <c r="C96" t="n">
-        <v>0.6047031796439619</v>
+        <v>0.6623066628222427</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5134425833131991</v>
+        <v>0.6248276450836094</v>
       </c>
       <c r="E96" t="n">
-        <v>0.6133183447770467</v>
+        <v>0.6659643814881866</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.5599939724894363</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2365,19 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.5099309055139511</v>
+        <v>0.6387044508505654</v>
       </c>
       <c r="C97" t="n">
-        <v>0.6051117659187778</v>
+        <v>0.662332920708401</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5133467335672945</v>
+        <v>0.6248457925648482</v>
       </c>
       <c r="E97" t="n">
-        <v>0.6136152733742218</v>
+        <v>0.6662868336892089</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.5595055806780165</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2385,19 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.509202529339232</v>
+        <v>0.6386434300346793</v>
       </c>
       <c r="C98" t="n">
-        <v>0.6049137365760273</v>
+        <v>0.6624887391058124</v>
       </c>
       <c r="D98" t="n">
-        <v>0.5140117705520462</v>
+        <v>0.6247049828214792</v>
       </c>
       <c r="E98" t="n">
-        <v>0.6137846297935436</v>
+        <v>0.6664929336032076</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.5590195541558918</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2405,19 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.5081236168009625</v>
+        <v>0.6386334015721635</v>
       </c>
       <c r="C99" t="n">
-        <v>0.6053649988548686</v>
+        <v>0.6628218670254705</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5135543793622543</v>
+        <v>0.6245887284507112</v>
       </c>
       <c r="E99" t="n">
-        <v>0.6130232219870646</v>
+        <v>0.666770060284003</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.5585425133590961</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2425,19 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.5083512354886537</v>
+        <v>0.6385507514119751</v>
       </c>
       <c r="C100" t="n">
-        <v>0.6050385830137585</v>
+        <v>0.6630504976474452</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5144142382293099</v>
+        <v>0.6246082002979432</v>
       </c>
       <c r="E100" t="n">
-        <v>0.6139995791481727</v>
+        <v>0.6670483061681746</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.5580613353852977</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2445,19 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.5077304498578014</v>
+        <v>0.638551917310558</v>
       </c>
       <c r="C101" t="n">
-        <v>0.6058360233830971</v>
+        <v>0.6631254191781032</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5147781230135777</v>
+        <v>0.6245329035739087</v>
       </c>
       <c r="E101" t="n">
-        <v>0.6146325412426318</v>
+        <v>0.6673645865087348</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.557585441997711</v>
       </c>
     </row>
     <row r="102">
@@ -2160,16 +2465,19 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.5078874513150446</v>
+        <v>0.6386496227862801</v>
       </c>
       <c r="C102" t="n">
-        <v>0.6062331956819161</v>
+        <v>0.6632435975380624</v>
       </c>
       <c r="D102" t="n">
-        <v>0.5143498733722657</v>
+        <v>0.6242231825519756</v>
       </c>
       <c r="E102" t="n">
-        <v>0.6144535761889816</v>
+        <v>0.6676597191342654</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.5571173150058611</v>
       </c>
     </row>
     <row r="103">
@@ -2177,16 +2485,19 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.5081531628186962</v>
+        <v>0.63875261439935</v>
       </c>
       <c r="C103" t="n">
-        <v>0.6063486826866653</v>
+        <v>0.6633738341702425</v>
       </c>
       <c r="D103" t="n">
-        <v>0.5150994058042455</v>
+        <v>0.6241439304052826</v>
       </c>
       <c r="E103" t="n">
-        <v>0.6148236592705808</v>
+        <v>0.6677614699779407</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.5566521635850312</v>
       </c>
     </row>
     <row r="104">
@@ -2194,16 +2505,19 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.5084518413924891</v>
+        <v>0.6388452824288107</v>
       </c>
       <c r="C104" t="n">
-        <v>0.6060422410458463</v>
+        <v>0.6634684515879121</v>
       </c>
       <c r="D104" t="n">
-        <v>0.5152113717942923</v>
+        <v>0.6240387554604439</v>
       </c>
       <c r="E104" t="n">
-        <v>0.6146069667749885</v>
+        <v>0.6679227457431077</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.5561873555325161</v>
       </c>
     </row>
     <row r="105">
@@ -2211,16 +2525,19 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.5081144791475076</v>
+        <v>0.6387302522928077</v>
       </c>
       <c r="C105" t="n">
-        <v>0.6061961824877925</v>
+        <v>0.6635034436469305</v>
       </c>
       <c r="D105" t="n">
-        <v>0.5152263120372474</v>
+        <v>0.6238463661481466</v>
       </c>
       <c r="E105" t="n">
-        <v>0.6142400550731102</v>
+        <v>0.6681443070339028</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.5557293282180982</v>
       </c>
     </row>
     <row r="106">
@@ -2228,16 +2545,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.5086567311433174</v>
+        <v>0.638789532339987</v>
       </c>
       <c r="C106" t="n">
-        <v>0.606728766756342</v>
+        <v>0.6636753860239742</v>
       </c>
       <c r="D106" t="n">
-        <v>0.5152732056722139</v>
+        <v>0.6239132683962032</v>
       </c>
       <c r="E106" t="n">
-        <v>0.6149630045971652</v>
+        <v>0.6682915112343284</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.555274690019636</v>
       </c>
     </row>
     <row r="107">
@@ -2245,16 +2565,19 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.5077318004602929</v>
+        <v>0.6386825166653181</v>
       </c>
       <c r="C107" t="n">
-        <v>0.6072879666511111</v>
+        <v>0.6639696765997082</v>
       </c>
       <c r="D107" t="n">
-        <v>0.5158160094313223</v>
+        <v>0.6236294251955492</v>
       </c>
       <c r="E107" t="n">
-        <v>0.6148315946548459</v>
+        <v>0.6685441596557407</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.5548216494465207</v>
       </c>
     </row>
     <row r="108">
@@ -2262,16 +2585,19 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.5076627019023116</v>
+        <v>0.6386333257357524</v>
       </c>
       <c r="C108" t="n">
-        <v>0.6074772456818018</v>
+        <v>0.664058680563312</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5160492424537415</v>
+        <v>0.6234019314366441</v>
       </c>
       <c r="E108" t="n">
-        <v>0.6156883186437481</v>
+        <v>0.6687299135678695</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.5543676650566289</v>
       </c>
     </row>
     <row r="109">
@@ -2279,16 +2605,19 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.5066741126682002</v>
+        <v>0.6385783383126656</v>
       </c>
       <c r="C109" t="n">
-        <v>0.6070214278380263</v>
+        <v>0.664186923359416</v>
       </c>
       <c r="D109" t="n">
-        <v>0.5171233610756928</v>
+        <v>0.6233981848244925</v>
       </c>
       <c r="E109" t="n">
-        <v>0.6168029494022083</v>
+        <v>0.6690232756747586</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.5539244437270088</v>
       </c>
     </row>
     <row r="110">
@@ -2296,16 +2625,19 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.5061618008921978</v>
+        <v>0.6386091955045743</v>
       </c>
       <c r="C110" t="n">
-        <v>0.6066275312813223</v>
+        <v>0.6643617409370021</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5172670348825779</v>
+        <v>0.6232861789936415</v>
       </c>
       <c r="E110" t="n">
-        <v>0.6178398437629272</v>
+        <v>0.6692681393027815</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.5534795759111013</v>
       </c>
     </row>
     <row r="111">
@@ -2313,16 +2645,19 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.5075203357689997</v>
+        <v>0.638828237150838</v>
       </c>
       <c r="C111" t="n">
-        <v>0.6068030474009858</v>
+        <v>0.664595866469406</v>
       </c>
       <c r="D111" t="n">
-        <v>0.5177352770519528</v>
+        <v>0.6231849756083386</v>
       </c>
       <c r="E111" t="n">
-        <v>0.6168461378148253</v>
+        <v>0.6696929428230589</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.5530435515504891</v>
       </c>
     </row>
     <row r="112">
@@ -2330,16 +2665,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.5079980147134373</v>
+        <v>0.6388702791333801</v>
       </c>
       <c r="C112" t="n">
-        <v>0.6070608775139269</v>
+        <v>0.6648661289464772</v>
       </c>
       <c r="D112" t="n">
-        <v>0.5169041686342839</v>
+        <v>0.6231508598787647</v>
       </c>
       <c r="E112" t="n">
-        <v>0.6171458262339898</v>
+        <v>0.6698986889675054</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.55260905247249</v>
       </c>
     </row>
     <row r="113">
@@ -2347,16 +2685,19 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.5076136095877571</v>
+        <v>0.6388942297294732</v>
       </c>
       <c r="C113" t="n">
-        <v>0.6068940739459074</v>
+        <v>0.6649971604764187</v>
       </c>
       <c r="D113" t="n">
-        <v>0.5174337913692779</v>
+        <v>0.6230453838508334</v>
       </c>
       <c r="E113" t="n">
-        <v>0.6174808337744969</v>
+        <v>0.6702135848026005</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.5521753342014127</v>
       </c>
     </row>
     <row r="114">
@@ -2364,16 +2705,19 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.5084224577354409</v>
+        <v>0.6388616208247242</v>
       </c>
       <c r="C114" t="n">
-        <v>0.607362446636192</v>
+        <v>0.665241812547811</v>
       </c>
       <c r="D114" t="n">
-        <v>0.5167170921840818</v>
+        <v>0.6229436436127969</v>
       </c>
       <c r="E114" t="n">
-        <v>0.617720633396986</v>
+        <v>0.6703176783187015</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.5517464923807892</v>
       </c>
     </row>
     <row r="115">
@@ -2381,16 +2725,19 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.5075473571165843</v>
+        <v>0.638944574886626</v>
       </c>
       <c r="C115" t="n">
-        <v>0.6080849271499031</v>
+        <v>0.6655625690582048</v>
       </c>
       <c r="D115" t="n">
-        <v>0.5164727018049725</v>
+        <v>0.6229537211386361</v>
       </c>
       <c r="E115" t="n">
-        <v>0.61753837323033</v>
+        <v>0.670412338858249</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.5513222704940897</v>
       </c>
     </row>
     <row r="116">
@@ -2398,16 +2745,19 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.5068107102834758</v>
+        <v>0.6388940763830855</v>
       </c>
       <c r="C116" t="n">
-        <v>0.6084301563700033</v>
+        <v>0.6657679582235529</v>
       </c>
       <c r="D116" t="n">
-        <v>0.5160429919165069</v>
+        <v>0.6228701537736345</v>
       </c>
       <c r="E116" t="n">
-        <v>0.6181201326750877</v>
+        <v>0.670767071673241</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.5509017941919455</v>
       </c>
     </row>
     <row r="117">
@@ -2415,16 +2765,19 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.5070439322384916</v>
+        <v>0.6388491777204665</v>
       </c>
       <c r="C117" t="n">
-        <v>0.6088555794178914</v>
+        <v>0.6657856958245659</v>
       </c>
       <c r="D117" t="n">
-        <v>0.5163892199336004</v>
+        <v>0.6228151460059008</v>
       </c>
       <c r="E117" t="n">
-        <v>0.6188624760719817</v>
+        <v>0.6709319317667005</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.5504832063340641</v>
       </c>
     </row>
     <row r="118">
@@ -2432,16 +2785,19 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.5064726306506365</v>
+        <v>0.63886454963715</v>
       </c>
       <c r="C118" t="n">
-        <v>0.6098578262078076</v>
+        <v>0.6660404362893201</v>
       </c>
       <c r="D118" t="n">
-        <v>0.5163269217032698</v>
+        <v>0.6228553568932137</v>
       </c>
       <c r="E118" t="n">
-        <v>0.6186048588202879</v>
+        <v>0.6709142971393972</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.5500671330830362</v>
       </c>
     </row>
     <row r="119">
@@ -2449,16 +2805,19 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.5062715223719161</v>
+        <v>0.6389008966604399</v>
       </c>
       <c r="C119" t="n">
-        <v>0.6102152035697672</v>
+        <v>0.6663217302325217</v>
       </c>
       <c r="D119" t="n">
-        <v>0.5158025870523091</v>
+        <v>0.6227719157246353</v>
       </c>
       <c r="E119" t="n">
-        <v>0.6182695891417291</v>
+        <v>0.6712909600689977</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.5496526911838615</v>
       </c>
     </row>
     <row r="120">
@@ -2466,16 +2825,19 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.5054235932761146</v>
+        <v>0.6388620590652375</v>
       </c>
       <c r="C120" t="n">
-        <v>0.6099744596974054</v>
+        <v>0.6664990990902211</v>
       </c>
       <c r="D120" t="n">
-        <v>0.516388174299199</v>
+        <v>0.6228491447799387</v>
       </c>
       <c r="E120" t="n">
-        <v>0.6178122561349848</v>
+        <v>0.6713817652930065</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.5492426846891589</v>
       </c>
     </row>
     <row r="121">
@@ -2483,16 +2845,19 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.5052712121731591</v>
+        <v>0.6389524749810521</v>
       </c>
       <c r="C121" t="n">
-        <v>0.6100538570223775</v>
+        <v>0.6667334086964308</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5167039294343778</v>
+        <v>0.6226493511489807</v>
       </c>
       <c r="E121" t="n">
-        <v>0.6182489718924021</v>
+        <v>0.6716174184767247</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.5488333608743549</v>
       </c>
     </row>
     <row r="122">
@@ -2500,16 +2865,19 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.5047867943708939</v>
+        <v>0.6388724163641293</v>
       </c>
       <c r="C122" t="n">
-        <v>0.6101371812333816</v>
+        <v>0.6670419882468829</v>
       </c>
       <c r="D122" t="n">
-        <v>0.5166324199930852</v>
+        <v>0.6225008419750661</v>
       </c>
       <c r="E122" t="n">
-        <v>0.6188037308745852</v>
+        <v>0.6718636976281425</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.5484316869809204</v>
       </c>
     </row>
     <row r="123">
@@ -2517,16 +2885,19 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.5051405585272005</v>
+        <v>0.6389837776955465</v>
       </c>
       <c r="C123" t="n">
-        <v>0.610409700829876</v>
+        <v>0.667396635768138</v>
       </c>
       <c r="D123" t="n">
-        <v>0.5157152487686475</v>
+        <v>0.622460233749299</v>
       </c>
       <c r="E123" t="n">
-        <v>0.6190418538329008</v>
+        <v>0.6720586158469342</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.5480317886768289</v>
       </c>
     </row>
     <row r="124">
@@ -2534,16 +2905,19 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.5048219805836111</v>
+        <v>0.6391031837394516</v>
       </c>
       <c r="C124" t="n">
-        <v>0.6103208261772017</v>
+        <v>0.6675992254603574</v>
       </c>
       <c r="D124" t="n">
-        <v>0.5150245350588636</v>
+        <v>0.6222377694475056</v>
       </c>
       <c r="E124" t="n">
-        <v>0.6188211959457426</v>
+        <v>0.6722597545131833</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.5476334609273998</v>
       </c>
     </row>
     <row r="125">
@@ -2551,16 +2925,19 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.5053531533378811</v>
+        <v>0.6389987733586736</v>
       </c>
       <c r="C125" t="n">
-        <v>0.6105321072056639</v>
+        <v>0.6677277617089172</v>
       </c>
       <c r="D125" t="n">
-        <v>0.5153331312817195</v>
+        <v>0.6221698497290455</v>
       </c>
       <c r="E125" t="n">
-        <v>0.6190879130516602</v>
+        <v>0.6724107238979165</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.5472365651641884</v>
       </c>
     </row>
     <row r="126">
@@ -2568,16 +2945,19 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.5059976232917599</v>
+        <v>0.6388730869758257</v>
       </c>
       <c r="C126" t="n">
-        <v>0.6109014168472684</v>
+        <v>0.6678492258189525</v>
       </c>
       <c r="D126" t="n">
-        <v>0.5153293294641312</v>
+        <v>0.6218732688578286</v>
       </c>
       <c r="E126" t="n">
-        <v>0.619272261552347</v>
+        <v>0.6725188573774937</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.5468461068835651</v>
       </c>
     </row>
     <row r="127">
@@ -2585,16 +2965,19 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.5062026773308435</v>
+        <v>0.638764550577412</v>
       </c>
       <c r="C127" t="n">
-        <v>0.6112307334862377</v>
+        <v>0.6679561555118937</v>
       </c>
       <c r="D127" t="n">
-        <v>0.5156618175457899</v>
+        <v>0.6217152072636138</v>
       </c>
       <c r="E127" t="n">
-        <v>0.6198014022112102</v>
+        <v>0.6728584905177752</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.5464614881161521</v>
       </c>
     </row>
     <row r="128">
@@ -2602,16 +2985,19 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.5061836487311759</v>
+        <v>0.6389269125631459</v>
       </c>
       <c r="C128" t="n">
-        <v>0.6112447190944436</v>
+        <v>0.6681734477102792</v>
       </c>
       <c r="D128" t="n">
-        <v>0.5160849086632748</v>
+        <v>0.6215784357265319</v>
       </c>
       <c r="E128" t="n">
-        <v>0.6198604829913912</v>
+        <v>0.6730531707360881</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0.5460739772106767</v>
       </c>
     </row>
     <row r="129">
@@ -2619,16 +3005,19 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.5064590722355724</v>
+        <v>0.6388597400343545</v>
       </c>
       <c r="C129" t="n">
-        <v>0.6112650653796287</v>
+        <v>0.6683420725748093</v>
       </c>
       <c r="D129" t="n">
-        <v>0.5167410420118257</v>
+        <v>0.621417494860934</v>
       </c>
       <c r="E129" t="n">
-        <v>0.6210565838925501</v>
+        <v>0.6734064444312887</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0.5456878541876813</v>
       </c>
     </row>
     <row r="130">
@@ -2636,16 +3025,19 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.5069068847060522</v>
+        <v>0.638808065211087</v>
       </c>
       <c r="C130" t="n">
-        <v>0.6109872426262066</v>
+        <v>0.6686438459667596</v>
       </c>
       <c r="D130" t="n">
-        <v>0.5169090704994617</v>
+        <v>0.6212989490506544</v>
       </c>
       <c r="E130" t="n">
-        <v>0.6205281472194837</v>
+        <v>0.6735827201132284</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.5453050840350967</v>
       </c>
     </row>
     <row r="131">
@@ -2653,16 +3045,19 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.506470602079495</v>
+        <v>0.6388264902600396</v>
       </c>
       <c r="C131" t="n">
-        <v>0.6114791639618522</v>
+        <v>0.6687584335408624</v>
       </c>
       <c r="D131" t="n">
-        <v>0.5172304966503318</v>
+        <v>0.6211590047113674</v>
       </c>
       <c r="E131" t="n">
-        <v>0.6207127888607453</v>
+        <v>0.6736892330037032</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0.5449281782649036</v>
       </c>
     </row>
     <row r="132">
@@ -2670,16 +3065,19 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.506405471918003</v>
+        <v>0.638682695735826</v>
       </c>
       <c r="C132" t="n">
-        <v>0.6117396059384324</v>
+        <v>0.6689172393030874</v>
       </c>
       <c r="D132" t="n">
-        <v>0.5165285209461674</v>
+        <v>0.6209156915165001</v>
       </c>
       <c r="E132" t="n">
-        <v>0.6205247671703161</v>
+        <v>0.6738980753918387</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0.5445550415005583</v>
       </c>
     </row>
     <row r="133">
@@ -2687,16 +3085,19 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.5065392783812027</v>
+        <v>0.6386409691093384</v>
       </c>
       <c r="C133" t="n">
-        <v>0.611724732955216</v>
+        <v>0.6691935626473681</v>
       </c>
       <c r="D133" t="n">
-        <v>0.5164041645716484</v>
+        <v>0.6208763492832376</v>
       </c>
       <c r="E133" t="n">
-        <v>0.6197212530804884</v>
+        <v>0.6740270047081395</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0.5441828327371994</v>
       </c>
     </row>
     <row r="134">
@@ -2704,16 +3105,19 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.5075841565130805</v>
+        <v>0.6385536887679126</v>
       </c>
       <c r="C134" t="n">
-        <v>0.6118534839330986</v>
+        <v>0.6693186571822841</v>
       </c>
       <c r="D134" t="n">
-        <v>0.5168325030783173</v>
+        <v>0.6208098969379291</v>
       </c>
       <c r="E134" t="n">
-        <v>0.6202861408897453</v>
+        <v>0.6742461657620078</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0.5438105174123308</v>
       </c>
     </row>
     <row r="135">
@@ -2721,16 +3125,19 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.5071570351430384</v>
+        <v>0.6386696957514197</v>
       </c>
       <c r="C135" t="n">
-        <v>0.6121016187259883</v>
+        <v>0.6694589321755137</v>
       </c>
       <c r="D135" t="n">
-        <v>0.5169243455610164</v>
+        <v>0.620736353803464</v>
       </c>
       <c r="E135" t="n">
-        <v>0.6207206987442957</v>
+        <v>0.6745309651842658</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0.5434444216759079</v>
       </c>
     </row>
     <row r="136">
@@ -2738,16 +3145,19 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.5079209266688492</v>
+        <v>0.6387126575790828</v>
       </c>
       <c r="C136" t="n">
-        <v>0.6125369697170591</v>
+        <v>0.6695783430537338</v>
       </c>
       <c r="D136" t="n">
-        <v>0.5172118040938385</v>
+        <v>0.6205924254429742</v>
       </c>
       <c r="E136" t="n">
-        <v>0.6211624300471933</v>
+        <v>0.6748520025914055</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0.5430858224053783</v>
       </c>
     </row>
     <row r="137">
@@ -2755,16 +3165,19 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.5079448107682003</v>
+        <v>0.6385677505259905</v>
       </c>
       <c r="C137" t="n">
-        <v>0.6126416128712096</v>
+        <v>0.6697011777669444</v>
       </c>
       <c r="D137" t="n">
-        <v>0.517168615572495</v>
+        <v>0.6204700162775063</v>
       </c>
       <c r="E137" t="n">
-        <v>0.621075903388016</v>
+        <v>0.6749806682234307</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.542721167949348</v>
       </c>
     </row>
     <row r="138">
@@ -2772,16 +3185,19 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.5081591034707725</v>
+        <v>0.6385141984248935</v>
       </c>
       <c r="C138" t="n">
-        <v>0.6124611944957221</v>
+        <v>0.669984684067691</v>
       </c>
       <c r="D138" t="n">
-        <v>0.5172623432841466</v>
+        <v>0.6203748816602663</v>
       </c>
       <c r="E138" t="n">
-        <v>0.6208554558284421</v>
+        <v>0.6750531254024322</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.542362582851437</v>
       </c>
     </row>
     <row r="139">
@@ -2789,16 +3205,19 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.507848088501059</v>
+        <v>0.6384586378000574</v>
       </c>
       <c r="C139" t="n">
-        <v>0.6123430743484717</v>
+        <v>0.6701481992140106</v>
       </c>
       <c r="D139" t="n">
-        <v>0.5171768401703229</v>
+        <v>0.6203576894858166</v>
       </c>
       <c r="E139" t="n">
-        <v>0.6202951750600858</v>
+        <v>0.6751664747874541</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.5420068117600791</v>
       </c>
     </row>
     <row r="140">
@@ -2806,16 +3225,19 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.5084893342325013</v>
+        <v>0.6385530452363731</v>
       </c>
       <c r="C140" t="n">
-        <v>0.612345130367397</v>
+        <v>0.6703398646323677</v>
       </c>
       <c r="D140" t="n">
-        <v>0.5167736652323061</v>
+        <v>0.6203425902448159</v>
       </c>
       <c r="E140" t="n">
-        <v>0.6197940424614401</v>
+        <v>0.6753832292593464</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.5416518759002198</v>
       </c>
     </row>
     <row r="141">
@@ -2823,16 +3245,19 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.507838304033448</v>
+        <v>0.6385814367201312</v>
       </c>
       <c r="C141" t="n">
-        <v>0.6123342151902595</v>
+        <v>0.6705467899290266</v>
       </c>
       <c r="D141" t="n">
-        <v>0.516779635710502</v>
+        <v>0.6201414015710646</v>
       </c>
       <c r="E141" t="n">
-        <v>0.6201893845843758</v>
+        <v>0.6756085258659963</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0.5412975270878221</v>
       </c>
     </row>
     <row r="142">
@@ -2840,16 +3265,19 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.5074860150384101</v>
+        <v>0.6385376082439987</v>
       </c>
       <c r="C142" t="n">
-        <v>0.6125187668166131</v>
+        <v>0.6706777003282494</v>
       </c>
       <c r="D142" t="n">
-        <v>0.5164733383297098</v>
+        <v>0.6200205358288129</v>
       </c>
       <c r="E142" t="n">
-        <v>0.6203403371912612</v>
+        <v>0.6758548927006293</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0.5409480164268002</v>
       </c>
     </row>
     <row r="143">
@@ -2857,16 +3285,19 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.507219860720047</v>
+        <v>0.6386062089894275</v>
       </c>
       <c r="C143" t="n">
-        <v>0.612464281842376</v>
+        <v>0.6707698788750592</v>
       </c>
       <c r="D143" t="n">
-        <v>0.5163471886512537</v>
+        <v>0.6198613076976031</v>
       </c>
       <c r="E143" t="n">
-        <v>0.6202211394903564</v>
+        <v>0.6759245690786131</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0.5406017883514244</v>
       </c>
     </row>
     <row r="144">
@@ -2874,16 +3305,19 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.5072864833960716</v>
+        <v>0.6385511702617315</v>
       </c>
       <c r="C144" t="n">
-        <v>0.6127703842779653</v>
+        <v>0.6709386745082152</v>
       </c>
       <c r="D144" t="n">
-        <v>0.5164761411335168</v>
+        <v>0.6197265967256985</v>
       </c>
       <c r="E144" t="n">
-        <v>0.6198608339414624</v>
+        <v>0.676086555307687</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0.5402584732361227</v>
       </c>
     </row>
     <row r="145">
@@ -2891,16 +3325,19 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.506872136533798</v>
+        <v>0.6386740828237951</v>
       </c>
       <c r="C145" t="n">
-        <v>0.6125687400029679</v>
+        <v>0.6710799199338523</v>
       </c>
       <c r="D145" t="n">
-        <v>0.5171653722794528</v>
+        <v>0.6196747563539805</v>
       </c>
       <c r="E145" t="n">
-        <v>0.6200221670302498</v>
+        <v>0.6763622398355823</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0.5399157320675858</v>
       </c>
     </row>
     <row r="146">
@@ -2908,16 +3345,19 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.5075355146482932</v>
+        <v>0.6388102781379962</v>
       </c>
       <c r="C146" t="n">
-        <v>0.6127472271025094</v>
+        <v>0.6712678722035884</v>
       </c>
       <c r="D146" t="n">
-        <v>0.5165134397752806</v>
+        <v>0.6195693438013458</v>
       </c>
       <c r="E146" t="n">
-        <v>0.619929004713513</v>
+        <v>0.6764563306910999</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0.5395778874366272</v>
       </c>
     </row>
     <row r="147">
@@ -2925,16 +3365,19 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.5070140343144893</v>
+        <v>0.6387938661534479</v>
       </c>
       <c r="C147" t="n">
-        <v>0.613184169486087</v>
+        <v>0.6713638767679986</v>
       </c>
       <c r="D147" t="n">
-        <v>0.5160455087892278</v>
+        <v>0.6195047840678275</v>
       </c>
       <c r="E147" t="n">
-        <v>0.6206878947399771</v>
+        <v>0.6765819307914995</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0.5392373869579024</v>
       </c>
     </row>
     <row r="148">
@@ -2942,16 +3385,19 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.5074649979965369</v>
+        <v>0.6389437240428912</v>
       </c>
       <c r="C148" t="n">
-        <v>0.6135138310025565</v>
+        <v>0.6714020498862543</v>
       </c>
       <c r="D148" t="n">
-        <v>0.5160177999117009</v>
+        <v>0.619318151969615</v>
       </c>
       <c r="E148" t="n">
-        <v>0.6213599910259869</v>
+        <v>0.6766831979911763</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0.5389009843858144</v>
       </c>
     </row>
     <row r="149">
@@ -2959,16 +3405,19 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.5069731378713594</v>
+        <v>0.6389399281340435</v>
       </c>
       <c r="C149" t="n">
-        <v>0.6136374268329088</v>
+        <v>0.6714394724063892</v>
       </c>
       <c r="D149" t="n">
-        <v>0.5155387850925666</v>
+        <v>0.6191089276930007</v>
       </c>
       <c r="E149" t="n">
-        <v>0.6221731318262914</v>
+        <v>0.6769042201339881</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0.5385690788756323</v>
       </c>
     </row>
     <row r="150">
@@ -2976,16 +3425,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.5067160476621646</v>
+        <v>0.6387824938705854</v>
       </c>
       <c r="C150" t="n">
-        <v>0.6138443205811523</v>
+        <v>0.6716027726684535</v>
       </c>
       <c r="D150" t="n">
-        <v>0.5151531348105356</v>
+        <v>0.6189675719672685</v>
       </c>
       <c r="E150" t="n">
-        <v>0.6220460595962065</v>
+        <v>0.6769676611432652</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0.5382354631950889</v>
       </c>
     </row>
     <row r="151">
@@ -2993,16 +3445,19 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.5065493285818036</v>
+        <v>0.6387643599168771</v>
       </c>
       <c r="C151" t="n">
-        <v>0.6137260268912581</v>
+        <v>0.6717164786254969</v>
       </c>
       <c r="D151" t="n">
-        <v>0.5151768971865336</v>
+        <v>0.6188564498662776</v>
       </c>
       <c r="E151" t="n">
-        <v>0.6222697824569169</v>
+        <v>0.6771987076240865</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0.5379079194119323</v>
       </c>
     </row>
     <row r="152">
@@ -3010,16 +3465,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.5067179299813481</v>
+        <v>0.6387965024322375</v>
       </c>
       <c r="C152" t="n">
-        <v>0.6142523660178804</v>
+        <v>0.671813946649386</v>
       </c>
       <c r="D152" t="n">
-        <v>0.5159694446434726</v>
+        <v>0.6187641138380174</v>
       </c>
       <c r="E152" t="n">
-        <v>0.623040552053836</v>
+        <v>0.6773596380144788</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0.5375851818438458</v>
       </c>
     </row>
     <row r="153">
@@ -3027,16 +3485,19 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.5067254794463917</v>
+        <v>0.6390040372950444</v>
       </c>
       <c r="C153" t="n">
-        <v>0.6144065223967202</v>
+        <v>0.6718902177962616</v>
       </c>
       <c r="D153" t="n">
-        <v>0.5162514153297535</v>
+        <v>0.6185140874268302</v>
       </c>
       <c r="E153" t="n">
-        <v>0.6230869656416915</v>
+        <v>0.6776298908548719</v>
+      </c>
+      <c r="F153" t="n">
+        <v>0.5372611354890946</v>
       </c>
     </row>
     <row r="154">
@@ -3044,16 +3505,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.5066590805227315</v>
+        <v>0.6390030910270685</v>
       </c>
       <c r="C154" t="n">
-        <v>0.614576697682767</v>
+        <v>0.6719938788705445</v>
       </c>
       <c r="D154" t="n">
-        <v>0.5163999071948109</v>
+        <v>0.6181848687723448</v>
       </c>
       <c r="E154" t="n">
-        <v>0.6233754310309998</v>
+        <v>0.6777499430403855</v>
+      </c>
+      <c r="F154" t="n">
+        <v>0.5369402619117173</v>
       </c>
     </row>
     <row r="155">
@@ -3061,16 +3525,19 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.5062355396964027</v>
+        <v>0.6391001170789377</v>
       </c>
       <c r="C155" t="n">
-        <v>0.6146371593705393</v>
+        <v>0.6720863906612407</v>
       </c>
       <c r="D155" t="n">
-        <v>0.5165396988576157</v>
+        <v>0.6181623094298344</v>
       </c>
       <c r="E155" t="n">
-        <v>0.6237500358423045</v>
+        <v>0.677876470652802</v>
+      </c>
+      <c r="F155" t="n">
+        <v>0.5366210639257417</v>
       </c>
     </row>
     <row r="156">
@@ -3078,16 +3545,19 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.5057250036845231</v>
+        <v>0.639138615608739</v>
       </c>
       <c r="C156" t="n">
-        <v>0.6149636508013805</v>
+        <v>0.672278809287538</v>
       </c>
       <c r="D156" t="n">
-        <v>0.5169013123947731</v>
+        <v>0.618093077341361</v>
       </c>
       <c r="E156" t="n">
-        <v>0.6238179517967674</v>
+        <v>0.6781106406931541</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0.5363061134684068</v>
       </c>
     </row>
     <row r="157">
@@ -3095,16 +3565,19 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.5056506650003882</v>
+        <v>0.6391606101248725</v>
       </c>
       <c r="C157" t="n">
-        <v>0.6151982155754697</v>
+        <v>0.6724461117151291</v>
       </c>
       <c r="D157" t="n">
-        <v>0.5169582659291592</v>
+        <v>0.6179206575893164</v>
       </c>
       <c r="E157" t="n">
-        <v>0.6235670801278655</v>
+        <v>0.6781860504052317</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0.5359889803031034</v>
       </c>
     </row>
     <row r="158">
@@ -3112,16 +3585,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.5055787392315538</v>
+        <v>0.6390187341389988</v>
       </c>
       <c r="C158" t="n">
-        <v>0.6155011520474033</v>
+        <v>0.6725670422335827</v>
       </c>
       <c r="D158" t="n">
-        <v>0.5177440100684797</v>
+        <v>0.6178333353520544</v>
       </c>
       <c r="E158" t="n">
-        <v>0.6238799123838824</v>
+        <v>0.6783725159240871</v>
+      </c>
+      <c r="F158" t="n">
+        <v>0.535675476588808</v>
       </c>
     </row>
     <row r="159">
@@ -3129,16 +3605,19 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5052073935933497</v>
+        <v>0.6391377347106888</v>
       </c>
       <c r="C159" t="n">
-        <v>0.615833465284619</v>
+        <v>0.6726309975516485</v>
       </c>
       <c r="D159" t="n">
-        <v>0.5178856700235105</v>
+        <v>0.6176454632324373</v>
       </c>
       <c r="E159" t="n">
-        <v>0.6237554259424017</v>
+        <v>0.6784978651933986</v>
+      </c>
+      <c r="F159" t="n">
+        <v>0.5353673709387022</v>
       </c>
     </row>
     <row r="160">
@@ -3146,16 +3625,19 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.5064058932444067</v>
+        <v>0.6391084993377987</v>
       </c>
       <c r="C160" t="n">
-        <v>0.6159607394733626</v>
+        <v>0.6727244204722759</v>
       </c>
       <c r="D160" t="n">
-        <v>0.5180361866985181</v>
+        <v>0.6174295319956677</v>
       </c>
       <c r="E160" t="n">
-        <v>0.624104344079065</v>
+        <v>0.678660039897123</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0.5350608107391774</v>
       </c>
     </row>
     <row r="161">
@@ -3163,16 +3645,19 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.5068790878442621</v>
+        <v>0.6390873710210646</v>
       </c>
       <c r="C161" t="n">
-        <v>0.6162239034039121</v>
+        <v>0.6729669928853015</v>
       </c>
       <c r="D161" t="n">
-        <v>0.5182566634662648</v>
+        <v>0.6173796405052721</v>
       </c>
       <c r="E161" t="n">
-        <v>0.6242043165187685</v>
+        <v>0.6789094714785634</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0.5347544370663951</v>
       </c>
     </row>
     <row r="162">
@@ -3180,16 +3665,19 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.5072110409727022</v>
+        <v>0.6390489740723494</v>
       </c>
       <c r="C162" t="n">
-        <v>0.6169797975184829</v>
+        <v>0.6731708184188341</v>
       </c>
       <c r="D162" t="n">
-        <v>0.5186752679151219</v>
+        <v>0.6172325431766068</v>
       </c>
       <c r="E162" t="n">
-        <v>0.6242311357229182</v>
+        <v>0.6790687681515821</v>
+      </c>
+      <c r="F162" t="n">
+        <v>0.5344508772362827</v>
       </c>
     </row>
     <row r="163">
@@ -3197,16 +3685,19 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.506983554183955</v>
+        <v>0.6390482042704057</v>
       </c>
       <c r="C163" t="n">
-        <v>0.6168198309549755</v>
+        <v>0.6733129244594541</v>
       </c>
       <c r="D163" t="n">
-        <v>0.5191253376435254</v>
+        <v>0.6171423498505084</v>
       </c>
       <c r="E163" t="n">
-        <v>0.6238542156260306</v>
+        <v>0.6791061754544958</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0.5341469536413717</v>
       </c>
     </row>
     <row r="164">
@@ -3214,16 +3705,19 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.5066994689762546</v>
+        <v>0.6389872154209216</v>
       </c>
       <c r="C164" t="n">
-        <v>0.6169431930689392</v>
+        <v>0.6734300438819826</v>
       </c>
       <c r="D164" t="n">
-        <v>0.5188497972769304</v>
+        <v>0.6169638137303616</v>
       </c>
       <c r="E164" t="n">
-        <v>0.6241354724087642</v>
+        <v>0.6792842867349923</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0.5338493709146862</v>
       </c>
     </row>
     <row r="165">
@@ -3231,16 +3725,19 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.5063829740164889</v>
+        <v>0.6390203160107059</v>
       </c>
       <c r="C165" t="n">
-        <v>0.6169937162520742</v>
+        <v>0.6734750367466289</v>
       </c>
       <c r="D165" t="n">
-        <v>0.5191647058756113</v>
+        <v>0.6168089648938719</v>
       </c>
       <c r="E165" t="n">
-        <v>0.6242673765599948</v>
+        <v>0.679454140496681</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0.5335513211116453</v>
       </c>
     </row>
     <row r="166">
@@ -3248,16 +3745,19 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.5064113511931614</v>
+        <v>0.6390265490644379</v>
       </c>
       <c r="C166" t="n">
-        <v>0.6169930164843124</v>
+        <v>0.6736188220504739</v>
       </c>
       <c r="D166" t="n">
-        <v>0.5190807770969925</v>
+        <v>0.6168376442901723</v>
       </c>
       <c r="E166" t="n">
-        <v>0.62435771314896</v>
+        <v>0.6797282759346067</v>
+      </c>
+      <c r="F166" t="n">
+        <v>0.5332545116496191</v>
       </c>
     </row>
     <row r="167">
@@ -3265,16 +3765,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.5065501792408333</v>
+        <v>0.6388269489060211</v>
       </c>
       <c r="C167" t="n">
-        <v>0.6164682709187405</v>
+        <v>0.6738136302519996</v>
       </c>
       <c r="D167" t="n">
-        <v>0.5190539716145843</v>
+        <v>0.6167205999818951</v>
       </c>
       <c r="E167" t="n">
-        <v>0.6250482004395493</v>
+        <v>0.6799983642199544</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0.5329641929776755</v>
       </c>
     </row>
     <row r="168">
@@ -3282,16 +3785,19 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.5065074870795152</v>
+        <v>0.6387330489267969</v>
       </c>
       <c r="C168" t="n">
-        <v>0.6162817515927288</v>
+        <v>0.6739893088364378</v>
       </c>
       <c r="D168" t="n">
-        <v>0.5191312796487491</v>
+        <v>0.6166886783505104</v>
       </c>
       <c r="E168" t="n">
-        <v>0.6252070834635532</v>
+        <v>0.6801607340711578</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0.5326706728584256</v>
       </c>
     </row>
     <row r="169">
@@ -3299,16 +3805,19 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.5061683354019408</v>
+        <v>0.6387522465235185</v>
       </c>
       <c r="C169" t="n">
-        <v>0.6166195217988973</v>
+        <v>0.6739963459152586</v>
       </c>
       <c r="D169" t="n">
-        <v>0.5192121170793467</v>
+        <v>0.6165821026521142</v>
       </c>
       <c r="E169" t="n">
-        <v>0.6248603599002729</v>
+        <v>0.6802700203182875</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0.5323837718208295</v>
       </c>
     </row>
     <row r="170">
@@ -3316,16 +3825,19 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.5058622646990617</v>
+        <v>0.6387981062954132</v>
       </c>
       <c r="C170" t="n">
-        <v>0.6165909321407392</v>
+        <v>0.6741047912724627</v>
       </c>
       <c r="D170" t="n">
-        <v>0.5186692813813931</v>
+        <v>0.6165312125108519</v>
       </c>
       <c r="E170" t="n">
-        <v>0.6249040540470016</v>
+        <v>0.6803944907916385</v>
+      </c>
+      <c r="F170" t="n">
+        <v>0.5320978135624093</v>
       </c>
     </row>
     <row r="171">
@@ -3333,16 +3845,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.5058408010621865</v>
+        <v>0.6388332476189158</v>
       </c>
       <c r="C171" t="n">
-        <v>0.6163979666217481</v>
+        <v>0.6741451072550484</v>
       </c>
       <c r="D171" t="n">
-        <v>0.5187255079087513</v>
+        <v>0.6164965245267741</v>
       </c>
       <c r="E171" t="n">
-        <v>0.6250192426809507</v>
+        <v>0.6805745791508937</v>
+      </c>
+      <c r="F171" t="n">
+        <v>0.5318099500684822</v>
       </c>
     </row>
     <row r="172">
@@ -3350,16 +3865,19 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.5054362158247305</v>
+        <v>0.6388040454293435</v>
       </c>
       <c r="C172" t="n">
-        <v>0.616403277378452</v>
+        <v>0.6742079320527816</v>
       </c>
       <c r="D172" t="n">
-        <v>0.5184133121038679</v>
+        <v>0.6162861450593508</v>
       </c>
       <c r="E172" t="n">
-        <v>0.6254135299814604</v>
+        <v>0.6805969667292093</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0.531523020249461</v>
       </c>
     </row>
     <row r="173">
@@ -3367,16 +3885,19 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.5054004290725713</v>
+        <v>0.6386692409663504</v>
       </c>
       <c r="C173" t="n">
-        <v>0.6165732350391807</v>
+        <v>0.6742682102363207</v>
       </c>
       <c r="D173" t="n">
-        <v>0.5186564705250195</v>
+        <v>0.6161604801777893</v>
       </c>
       <c r="E173" t="n">
-        <v>0.6253817648979429</v>
+        <v>0.6807562908718985</v>
+      </c>
+      <c r="F173" t="n">
+        <v>0.5312431356508521</v>
       </c>
     </row>
     <row r="174">
@@ -3384,16 +3905,19 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.5048958845127605</v>
+        <v>0.6386816844379652</v>
       </c>
       <c r="C174" t="n">
-        <v>0.6169630151482142</v>
+        <v>0.674364963255755</v>
       </c>
       <c r="D174" t="n">
-        <v>0.5182213058497135</v>
+        <v>0.6159309516387748</v>
       </c>
       <c r="E174" t="n">
-        <v>0.6253174929132046</v>
+        <v>0.6809381999677377</v>
+      </c>
+      <c r="F174" t="n">
+        <v>0.5309603924281955</v>
       </c>
     </row>
     <row r="175">
@@ -3401,16 +3925,19 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.5045129111961145</v>
+        <v>0.6385769484520324</v>
       </c>
       <c r="C175" t="n">
-        <v>0.6170988906856705</v>
+        <v>0.6744714628604317</v>
       </c>
       <c r="D175" t="n">
-        <v>0.5187201585590262</v>
+        <v>0.6158689337256698</v>
       </c>
       <c r="E175" t="n">
-        <v>0.6253942118759115</v>
+        <v>0.6810677275749348</v>
+      </c>
+      <c r="F175" t="n">
+        <v>0.5306785089071728</v>
       </c>
     </row>
     <row r="176">
@@ -3418,16 +3945,19 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.5040603394095928</v>
+        <v>0.6386402018072139</v>
       </c>
       <c r="C176" t="n">
-        <v>0.6173266652620439</v>
+        <v>0.6744821221892301</v>
       </c>
       <c r="D176" t="n">
-        <v>0.5190274272678931</v>
+        <v>0.6156528834975321</v>
       </c>
       <c r="E176" t="n">
-        <v>0.6256069854771602</v>
+        <v>0.6812441662043087</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0.5304014300021832</v>
       </c>
     </row>
     <row r="177">
@@ -3435,16 +3965,19 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.5043317633513069</v>
+        <v>0.6387512653963328</v>
       </c>
       <c r="C177" t="n">
-        <v>0.6171639259721811</v>
+        <v>0.6745334125317828</v>
       </c>
       <c r="D177" t="n">
-        <v>0.5186339216549911</v>
+        <v>0.6155441860490609</v>
       </c>
       <c r="E177" t="n">
-        <v>0.6261743744805051</v>
+        <v>0.6813710736405969</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0.5301268103641774</v>
       </c>
     </row>
     <row r="178">
@@ -3452,16 +3985,19 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.5041036882389408</v>
+        <v>0.6387757378019473</v>
       </c>
       <c r="C178" t="n">
-        <v>0.6174527737715827</v>
+        <v>0.6747281897012292</v>
       </c>
       <c r="D178" t="n">
-        <v>0.5185505636104947</v>
+        <v>0.6154536371111176</v>
       </c>
       <c r="E178" t="n">
-        <v>0.6265346905748876</v>
+        <v>0.6815084595351072</v>
+      </c>
+      <c r="F178" t="n">
+        <v>0.5298535876254474</v>
       </c>
     </row>
     <row r="179">
@@ -3469,16 +4005,19 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.5037885439016836</v>
+        <v>0.6386059682987609</v>
       </c>
       <c r="C179" t="n">
-        <v>0.6176353925585825</v>
+        <v>0.6748475785510978</v>
       </c>
       <c r="D179" t="n">
-        <v>0.5191446833209334</v>
+        <v>0.615462115761628</v>
       </c>
       <c r="E179" t="n">
-        <v>0.6268557156164738</v>
+        <v>0.6816308228994374</v>
+      </c>
+      <c r="F179" t="n">
+        <v>0.5295814584939839</v>
       </c>
     </row>
     <row r="180">
@@ -3486,16 +4025,19 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.503849509852955</v>
+        <v>0.6385018217178338</v>
       </c>
       <c r="C180" t="n">
-        <v>0.6176716156679227</v>
+        <v>0.6749417376816771</v>
       </c>
       <c r="D180" t="n">
-        <v>0.5192549362658306</v>
+        <v>0.6153726911952564</v>
       </c>
       <c r="E180" t="n">
-        <v>0.6269670625337683</v>
+        <v>0.6817708659636935</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0.5293114677043772</v>
       </c>
     </row>
     <row r="181">
@@ -3503,16 +4045,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.5041938422572082</v>
+        <v>0.6385207907852802</v>
       </c>
       <c r="C181" t="n">
-        <v>0.6178476602749658</v>
+        <v>0.6750231074520852</v>
       </c>
       <c r="D181" t="n">
-        <v>0.5198377587261425</v>
+        <v>0.6151235447841323</v>
       </c>
       <c r="E181" t="n">
-        <v>0.6275285156990795</v>
+        <v>0.6819637907093787</v>
+      </c>
+      <c r="F181" t="n">
+        <v>0.529044304770838</v>
       </c>
     </row>
     <row r="182">
@@ -3520,16 +4065,19 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.5043168680832202</v>
+        <v>0.638333525453042</v>
       </c>
       <c r="C182" t="n">
-        <v>0.6182569429880361</v>
+        <v>0.6751480725033414</v>
       </c>
       <c r="D182" t="n">
-        <v>0.5199647508004679</v>
+        <v>0.615086261740923</v>
       </c>
       <c r="E182" t="n">
-        <v>0.6275945475878422</v>
+        <v>0.6820684684444911</v>
+      </c>
+      <c r="F182" t="n">
+        <v>0.5287765242281612</v>
       </c>
     </row>
     <row r="183">
@@ -3537,16 +4085,19 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.5043577787838032</v>
+        <v>0.6383254540884973</v>
       </c>
       <c r="C183" t="n">
-        <v>0.6184252752054096</v>
+        <v>0.6752517546154064</v>
       </c>
       <c r="D183" t="n">
-        <v>0.5197443681337399</v>
+        <v>0.6148852858249196</v>
       </c>
       <c r="E183" t="n">
-        <v>0.6279374394586009</v>
+        <v>0.6822225125992583</v>
+      </c>
+      <c r="F183" t="n">
+        <v>0.5285096544434277</v>
       </c>
     </row>
     <row r="184">
@@ -3554,16 +4105,19 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.5044498209068664</v>
+        <v>0.6383702492974391</v>
       </c>
       <c r="C184" t="n">
-        <v>0.6187771269936146</v>
+        <v>0.6753044970352151</v>
       </c>
       <c r="D184" t="n">
-        <v>0.520237539049887</v>
+        <v>0.614814164026269</v>
       </c>
       <c r="E184" t="n">
-        <v>0.6280310748517897</v>
+        <v>0.6823769744226305</v>
+      </c>
+      <c r="F184" t="n">
+        <v>0.5282446950812267</v>
       </c>
     </row>
     <row r="185">
@@ -3571,16 +4125,19 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.5048871196685245</v>
+        <v>0.638379327678338</v>
       </c>
       <c r="C185" t="n">
-        <v>0.6186831334307067</v>
+        <v>0.6753794611606497</v>
       </c>
       <c r="D185" t="n">
-        <v>0.5205670838392517</v>
+        <v>0.6146937523985767</v>
       </c>
       <c r="E185" t="n">
-        <v>0.6278907675057799</v>
+        <v>0.6825087122486727</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0.5279846653234809</v>
       </c>
     </row>
     <row r="186">
@@ -3588,16 +4145,19 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.5045733898180973</v>
+        <v>0.6383812442424315</v>
       </c>
       <c r="C186" t="n">
-        <v>0.6185302371898137</v>
+        <v>0.6754691407586864</v>
       </c>
       <c r="D186" t="n">
-        <v>0.5208313935323853</v>
+        <v>0.6145653036875477</v>
       </c>
       <c r="E186" t="n">
-        <v>0.6285851754994164</v>
+        <v>0.682637774733585</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0.527722720509582</v>
       </c>
     </row>
     <row r="187">
@@ -3605,16 +4165,19 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.504726216254396</v>
+        <v>0.6382502097789342</v>
       </c>
       <c r="C187" t="n">
-        <v>0.6187406271475078</v>
+        <v>0.6755821000864939</v>
       </c>
       <c r="D187" t="n">
-        <v>0.5207441471636134</v>
+        <v>0.6145605777739417</v>
       </c>
       <c r="E187" t="n">
-        <v>0.6286277404751048</v>
+        <v>0.6826669283579663</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0.5274663867614502</v>
       </c>
     </row>
     <row r="188">
@@ -3622,16 +4185,19 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.504981678030099</v>
+        <v>0.6383366221970237</v>
       </c>
       <c r="C188" t="n">
-        <v>0.6188470915641175</v>
+        <v>0.6756242568059746</v>
       </c>
       <c r="D188" t="n">
-        <v>0.5206833761543025</v>
+        <v>0.614484500134596</v>
       </c>
       <c r="E188" t="n">
-        <v>0.6289054754066962</v>
+        <v>0.6826897572705474</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0.5272085568786966</v>
       </c>
     </row>
     <row r="189">
@@ -3639,16 +4205,19 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.5050917267965619</v>
+        <v>0.63836442240573</v>
       </c>
       <c r="C189" t="n">
-        <v>0.619082257692616</v>
+        <v>0.6757932826519085</v>
       </c>
       <c r="D189" t="n">
-        <v>0.5210047445183005</v>
+        <v>0.6143357009747784</v>
       </c>
       <c r="E189" t="n">
-        <v>0.6294213999311973</v>
+        <v>0.6829037110586854</v>
+      </c>
+      <c r="F189" t="n">
+        <v>0.5269526579250067</v>
       </c>
     </row>
     <row r="190">
@@ -3656,16 +4225,19 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.5052535911742646</v>
+        <v>0.6383743673619058</v>
       </c>
       <c r="C190" t="n">
-        <v>0.6194946581745373</v>
+        <v>0.6758839160081479</v>
       </c>
       <c r="D190" t="n">
-        <v>0.5211002196591099</v>
+        <v>0.614113595882795</v>
       </c>
       <c r="E190" t="n">
-        <v>0.6294667079180246</v>
+        <v>0.683014864941861</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0.526699760023397</v>
       </c>
     </row>
     <row r="191">
@@ -3673,16 +4245,19 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.5049567108223169</v>
+        <v>0.6384494282274698</v>
       </c>
       <c r="C191" t="n">
-        <v>0.6197463641282117</v>
+        <v>0.675986512699794</v>
       </c>
       <c r="D191" t="n">
-        <v>0.5213229473998385</v>
+        <v>0.6140180569833804</v>
       </c>
       <c r="E191" t="n">
-        <v>0.6295293591964737</v>
+        <v>0.6831966397468174</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0.5264492537104755</v>
       </c>
     </row>
     <row r="192">
@@ -3690,16 +4265,19 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.5056005737240504</v>
+        <v>0.6385077761395406</v>
       </c>
       <c r="C192" t="n">
-        <v>0.6200283684372285</v>
+        <v>0.6760827474772818</v>
       </c>
       <c r="D192" t="n">
-        <v>0.5208816877372388</v>
+        <v>0.613901013987225</v>
       </c>
       <c r="E192" t="n">
-        <v>0.6290118165853762</v>
+        <v>0.6834052265396255</v>
+      </c>
+      <c r="F192" t="n">
+        <v>0.5261995097927414</v>
       </c>
     </row>
     <row r="193">
@@ -3707,16 +4285,19 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.505843013506475</v>
+        <v>0.6385728971976701</v>
       </c>
       <c r="C193" t="n">
-        <v>0.6202654078422509</v>
+        <v>0.6760864295675451</v>
       </c>
       <c r="D193" t="n">
-        <v>0.5209499540984337</v>
+        <v>0.6137847670209952</v>
       </c>
       <c r="E193" t="n">
-        <v>0.6293242397265626</v>
+        <v>0.6835399837189795</v>
+      </c>
+      <c r="F193" t="n">
+        <v>0.5259514577372004</v>
       </c>
     </row>
     <row r="194">
@@ -3724,16 +4305,19 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.5057775579606841</v>
+        <v>0.6385591597448195</v>
       </c>
       <c r="C194" t="n">
-        <v>0.6206822003135526</v>
+        <v>0.6761747035602893</v>
       </c>
       <c r="D194" t="n">
-        <v>0.52067103490427</v>
+        <v>0.6136671524332244</v>
       </c>
       <c r="E194" t="n">
-        <v>0.6293002804551004</v>
+        <v>0.6835908955432937</v>
+      </c>
+      <c r="F194" t="n">
+        <v>0.5257027325297309</v>
       </c>
     </row>
     <row r="195">
@@ -3741,16 +4325,19 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.5059007085239682</v>
+        <v>0.6384447670251971</v>
       </c>
       <c r="C195" t="n">
-        <v>0.6210537086327763</v>
+        <v>0.6762484224957296</v>
       </c>
       <c r="D195" t="n">
-        <v>0.520762519090136</v>
+        <v>0.6135879077124978</v>
       </c>
       <c r="E195" t="n">
-        <v>0.6290594795732078</v>
+        <v>0.6836574456279244</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0.5254561477753049</v>
       </c>
     </row>
     <row r="196">
@@ -3758,16 +4345,19 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.5058630017138978</v>
+        <v>0.6385362483653451</v>
       </c>
       <c r="C196" t="n">
-        <v>0.6210598311500448</v>
+        <v>0.6763845227605765</v>
       </c>
       <c r="D196" t="n">
-        <v>0.5209194131534731</v>
+        <v>0.6133221965426349</v>
       </c>
       <c r="E196" t="n">
-        <v>0.629673434799382</v>
+        <v>0.6838810786438008</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0.5252102910299008</v>
       </c>
     </row>
     <row r="197">
@@ -3775,16 +4365,19 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.5056730226356534</v>
+        <v>0.6384780106459048</v>
       </c>
       <c r="C197" t="n">
-        <v>0.6211823018174198</v>
+        <v>0.6765012220945743</v>
       </c>
       <c r="D197" t="n">
-        <v>0.5210391633860787</v>
+        <v>0.6131796237686247</v>
       </c>
       <c r="E197" t="n">
-        <v>0.6290278282773858</v>
+        <v>0.6840816949848474</v>
+      </c>
+      <c r="F197" t="n">
+        <v>0.5249708141777316</v>
       </c>
     </row>
     <row r="198">
@@ -3792,16 +4385,19 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.5057618583852919</v>
+        <v>0.638335328487891</v>
       </c>
       <c r="C198" t="n">
-        <v>0.621507457365465</v>
+        <v>0.6765791250141829</v>
       </c>
       <c r="D198" t="n">
-        <v>0.5213626551337109</v>
+        <v>0.6131950515057084</v>
       </c>
       <c r="E198" t="n">
-        <v>0.6292759043147963</v>
+        <v>0.6841833719827606</v>
+      </c>
+      <c r="F198" t="n">
+        <v>0.5247288500541583</v>
       </c>
     </row>
     <row r="199">
@@ -3809,16 +4405,19 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.5053568454173507</v>
+        <v>0.6382766156011603</v>
       </c>
       <c r="C199" t="n">
-        <v>0.6213769738819435</v>
+        <v>0.6766386233128687</v>
       </c>
       <c r="D199" t="n">
-        <v>0.5218502583685756</v>
+        <v>0.6132193537847387</v>
       </c>
       <c r="E199" t="n">
-        <v>0.6290097067786561</v>
+        <v>0.6844007147102815</v>
+      </c>
+      <c r="F199" t="n">
+        <v>0.5244877893739498</v>
       </c>
     </row>
     <row r="200">
@@ -3826,16 +4425,19 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.5056679752999104</v>
+        <v>0.6382258477743755</v>
       </c>
       <c r="C200" t="n">
-        <v>0.6215614117786455</v>
+        <v>0.6768171377699852</v>
       </c>
       <c r="D200" t="n">
-        <v>0.5218367855942242</v>
+        <v>0.6130303425077643</v>
       </c>
       <c r="E200" t="n">
-        <v>0.6292928209008953</v>
+        <v>0.6845485818282773</v>
+      </c>
+      <c r="F200" t="n">
+        <v>0.5242486284869468</v>
       </c>
     </row>
     <row r="201">
@@ -3843,16 +4445,19 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.5054932329135278</v>
+        <v>0.6381587374545374</v>
       </c>
       <c r="C201" t="n">
-        <v>0.621422153863276</v>
+        <v>0.6769710080277466</v>
       </c>
       <c r="D201" t="n">
-        <v>0.5219557276661598</v>
+        <v>0.612982556683759</v>
       </c>
       <c r="E201" t="n">
-        <v>0.6289897672731108</v>
+        <v>0.6847518511662252</v>
+      </c>
+      <c r="F201" t="n">
+        <v>0.524008199978041</v>
       </c>
     </row>
     <row r="202">
@@ -3860,16 +4465,19 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>0.5056309636307559</v>
+        <v>0.638159212682271</v>
       </c>
       <c r="C202" t="n">
-        <v>0.6214293985735474</v>
+        <v>0.6770079483306407</v>
       </c>
       <c r="D202" t="n">
-        <v>0.5227159589631892</v>
+        <v>0.6129449856828402</v>
       </c>
       <c r="E202" t="n">
-        <v>0.6287048858778221</v>
+        <v>0.6849380801109906</v>
+      </c>
+      <c r="F202" t="n">
+        <v>0.5237734491527002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>